<commit_message>
Tasks have absolute dates
</commit_message>
<xml_diff>
--- a/outputs/PortfolioMarc_solutions.xlsx
+++ b/outputs/PortfolioMarc_solutions.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Finish Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Predecessors</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Successors</t>
         </is>
@@ -495,8 +505,18 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>08-01-2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>08-01-2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2, 3, 4</t>
         </is>
@@ -524,10 +544,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>08-01-2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>29-03-2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -555,10 +585,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>29-03-2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>17-06-2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -586,10 +626,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>17-06-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>05-09-2023</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -617,10 +667,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>05-09-2023</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>05-09-2023</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>3, 4, 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -633,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,10 +729,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Finish Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Predecessors</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Successors</t>
         </is>
@@ -698,8 +768,18 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>08-01-2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>08-01-2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2, 3, 4</t>
         </is>
@@ -727,10 +807,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>08-01-2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>29-03-2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -758,10 +848,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>08-01-2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>29-03-2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -789,10 +889,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>08-01-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>29-03-2023</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -820,10 +930,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>29-03-2023</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>29-03-2023</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>3, 4, 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -836,7 +956,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -872,10 +992,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Finish Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Predecessors</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Successors</t>
         </is>
@@ -901,8 +1031,18 @@
       <c r="E2" t="n">
         <v>10</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18-01-2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>18-01-2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2, 3, 4</t>
         </is>
@@ -930,10 +1070,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18-01-2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>08-04-2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -961,10 +1111,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>08-04-2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>27-06-2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -992,10 +1152,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>27-06-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>15-09-2023</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1023,10 +1193,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>15-09-2023</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>15-09-2023</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>3, 4, 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1039,7 +1219,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1075,10 +1255,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Finish Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Predecessors</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Successors</t>
         </is>
@@ -1104,8 +1294,18 @@
       <c r="E2" t="n">
         <v>10</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18-01-2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>18-01-2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2, 3, 4</t>
         </is>
@@ -1133,10 +1333,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18-01-2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>08-04-2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1164,10 +1374,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18-01-2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>08-04-2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1195,10 +1415,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18-01-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>08-04-2023</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1226,10 +1456,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>08-04-2023</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>08-04-2023</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>3, 4, 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1242,7 +1482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1278,10 +1518,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Finish Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Predecessors</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Successors</t>
         </is>
@@ -1307,8 +1557,18 @@
       <c r="E2" t="n">
         <v>20</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>28-01-2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>28-01-2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2, 3, 4</t>
         </is>
@@ -1336,10 +1596,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>28-01-2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>18-04-2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1367,10 +1637,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18-04-2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>07-07-2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1398,10 +1678,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>07-07-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>25-09-2023</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1429,10 +1719,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>25-09-2023</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>25-09-2023</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>3, 4, 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1445,7 +1745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,10 +1781,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Finish Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Predecessors</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Successors</t>
         </is>
@@ -1510,8 +1820,18 @@
       <c r="E2" t="n">
         <v>20</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>28-01-2023</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>28-01-2023</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2, 3, 4</t>
         </is>
@@ -1539,10 +1859,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>28-01-2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>18-04-2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1570,10 +1900,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>28-01-2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>18-04-2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1601,10 +1941,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>28-01-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>18-04-2023</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1632,10 +1982,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>18-04-2023</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>18-04-2023</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>3, 4, 5</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>